<commit_message>
pipe heat loss calculation updated; views added and updated; Code reformatted
</commit_message>
<xml_diff>
--- a/resources/parameters/Parameter.xlsx
+++ b/resources/parameters/Parameter.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\pbe1\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\pbe1\resources\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B27BB34-0559-49D3-A5F2-E48D9F17D957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F7FE9A-668A-4B95-BCC8-C804A0B6C732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameter" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
   <si>
     <t>Parameter</t>
   </si>
@@ -245,15 +245,6 @@
     <t>tolerabler Druckverlust allgemein (Pa/m)</t>
   </si>
   <si>
-    <t>Vorlauftemperatur (K)</t>
-  </si>
-  <si>
-    <t>Rücklauftemperatur (K)</t>
-  </si>
-  <si>
-    <t>Temperaturdelta Vor-Rücklauf (K)</t>
-  </si>
-  <si>
     <t>Netzauslegung_initial</t>
   </si>
   <si>
@@ -266,27 +257,15 @@
     <t>Rohrauswahl</t>
   </si>
   <si>
-    <t>PMR</t>
-  </si>
-  <si>
     <t>#Rohrparameter</t>
   </si>
   <si>
-    <t>Alternativer Rohrtyp</t>
-  </si>
-  <si>
-    <t>KMR</t>
-  </si>
-  <si>
     <t>Initiale Dämmung</t>
   </si>
   <si>
     <t>DS1</t>
   </si>
   <si>
-    <t>Initialer Rohrtyp</t>
-  </si>
-  <si>
     <t>Rohrrauheit k (mm)</t>
   </si>
   <si>
@@ -318,6 +297,33 @@
   </si>
   <si>
     <t>Annahme eines verhälnismäßig kleinen Duschraums bezogen auf die Gebäudegröße</t>
+  </si>
+  <si>
+    <t>Vorlauftemperatur Winter (K)</t>
+  </si>
+  <si>
+    <t>Rücklauftemperatur Winter (K)</t>
+  </si>
+  <si>
+    <t>Vorlauftemperatur Sommer (K)</t>
+  </si>
+  <si>
+    <t>Rücklauftemperatur Sommer (K)</t>
+  </si>
+  <si>
+    <t>75°C Vorlauftemperatur Auslegung</t>
+  </si>
+  <si>
+    <t>55°C Rücklauftemperatur Auslegung</t>
+  </si>
+  <si>
+    <t>55°C Rücklauftemperatur Sommer</t>
+  </si>
+  <si>
+    <t>65°C Vorlauftemperatur Sommer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,5°C Bodentemperaturen </t>
   </si>
 </sst>
 </file>
@@ -401,8 +407,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{515CD144-5CD8-4CAD-B4CD-DD51ABA4ED7A}" name="Tabelle1" displayName="Tabelle1" ref="A1:E50" totalsRowShown="0">
-  <autoFilter ref="A1:E50" xr:uid="{515CD144-5CD8-4CAD-B4CD-DD51ABA4ED7A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{515CD144-5CD8-4CAD-B4CD-DD51ABA4ED7A}" name="Tabelle1" displayName="Tabelle1" ref="A1:E49" totalsRowShown="0">
+  <autoFilter ref="A1:E49" xr:uid="{515CD144-5CD8-4CAD-B4CD-DD51ABA4ED7A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{384E1191-F8EA-48F3-B1EA-1167641B2694}" name="Kategorie"/>
     <tableColumn id="5" xr3:uid="{3DE239F4-2900-44F9-A341-275202F5AA90}" name="Parameter"/>
@@ -677,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1038,7 @@
         <v>0.5</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1134,10 +1140,13 @@
         <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C34" s="5">
         <v>348.15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1145,10 +1154,13 @@
         <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C35" s="5">
         <v>328.15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1156,10 +1168,13 @@
         <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="7">
-        <v>20</v>
+        <v>89</v>
+      </c>
+      <c r="C36" s="5">
+        <v>338.15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1167,10 +1182,13 @@
         <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C37" s="5">
-        <v>276.64999999999998</v>
+        <v>328.15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1178,10 +1196,13 @@
         <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C38" s="5">
-        <v>290.64999999999998</v>
+        <v>276.64999999999998</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1189,139 +1210,128 @@
         <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" t="s">
-        <v>23</v>
+        <v>79</v>
+      </c>
+      <c r="C39" s="5">
+        <v>290.64999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C40" s="6">
-        <v>3</v>
+        <v>0.8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
-      </c>
-      <c r="C41" s="2">
-        <v>974.98900000000003</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
+        <v>66</v>
+      </c>
+      <c r="C41" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C42" s="2">
-        <v>985.83690000000001</v>
+        <v>974.98900000000003</v>
       </c>
       <c r="D42" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="8">
+        <v>71</v>
+      </c>
+      <c r="C43" s="2">
+        <v>985.83690000000001</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="8">
         <f>0.38751610493371*0.00001</f>
         <v>3.8751610493371007E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="8">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="8">
         <f>0.51128491182691*0.00001</f>
         <v>5.1128491182691007E-6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="3"/>
-    </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" t="s">
-        <v>82</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="A46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="C48" s="5">
+        <v>0.01</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="7">
+        <v>77</v>
+      </c>
+      <c r="C49" s="7">
         <v>2320</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hinzufügen der Quellen. Einige fehlen noch, da müsste Tim gefragt werden
</commit_message>
<xml_diff>
--- a/resources/parameters/Parameter.xlsx
+++ b/resources/parameters/Parameter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\pbe1\resources\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\pbe1\resources\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F7FE9A-668A-4B95-BCC8-C804A0B6C732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B51BC00-B012-4056-9C87-E0577DDBF239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>Parameter</t>
   </si>
@@ -324,6 +324,48 @@
   </si>
   <si>
     <t xml:space="preserve">3,5°C Bodentemperaturen </t>
+  </si>
+  <si>
+    <t>Vorlesung 00 Hinweise zur Bearbeitung Folie 10 Punkt 7-9 Annahme Rohrrauheit</t>
+  </si>
+  <si>
+    <t>Vorlesung 04 Folie 9</t>
+  </si>
+  <si>
+    <t>Maximalwert</t>
+  </si>
+  <si>
+    <t>Vorlesung 02 Folie 10</t>
+  </si>
+  <si>
+    <t>Maximale Stromungsgeschwindigkeit auf Grund von Geräuschemissionen</t>
+  </si>
+  <si>
+    <t>Planungshandbuch Seite 128</t>
+  </si>
+  <si>
+    <t>Annahme Rohrrauheit</t>
+  </si>
+  <si>
+    <t>Reynolds-Zahl</t>
+  </si>
+  <si>
+    <t>Wir beginnen mit der günstigsten Insolationsstufe</t>
+  </si>
+  <si>
+    <t>17,5°C Bodentemperatur</t>
+  </si>
+  <si>
+    <t>Tim fragen</t>
+  </si>
+  <si>
+    <t>http://www.peacesoftware.de/einigewerte/wasser_dampf.html</t>
+  </si>
+  <si>
+    <t>Vorlesung 03 Folie 24 Beründung siehe Doku_all</t>
+  </si>
+  <si>
+    <t>https://www.kern-haus.de/ratgeber/baulexikon/satteldach/</t>
   </si>
 </sst>
 </file>
@@ -336,7 +378,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +390,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,10 +427,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -385,8 +443,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -685,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD47"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,6 +880,9 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
+      <c r="E8" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -981,6 +1045,9 @@
       <c r="C20" s="2">
         <v>1.1999</v>
       </c>
+      <c r="E20" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -992,6 +1059,9 @@
       <c r="C21" s="2">
         <v>1.351</v>
       </c>
+      <c r="E21" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1003,6 +1073,9 @@
       <c r="C22" s="5">
         <v>0.28000000000000003</v>
       </c>
+      <c r="E22" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1123,6 +1196,12 @@
       <c r="C32" s="7">
         <v>200</v>
       </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1134,6 +1213,12 @@
       <c r="C33" s="7">
         <v>300</v>
       </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1148,6 +1233,9 @@
       <c r="D34" t="s">
         <v>91</v>
       </c>
+      <c r="E34" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1162,6 +1250,9 @@
       <c r="D35" t="s">
         <v>92</v>
       </c>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1176,6 +1267,9 @@
       <c r="D36" t="s">
         <v>94</v>
       </c>
+      <c r="E36" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1190,6 +1284,9 @@
       <c r="D37" t="s">
         <v>93</v>
       </c>
+      <c r="E37" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1204,6 +1301,9 @@
       <c r="D38" t="s">
         <v>95</v>
       </c>
+      <c r="E38" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1215,6 +1315,12 @@
       <c r="C39" s="5">
         <v>290.64999999999998</v>
       </c>
+      <c r="D39" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1243,6 +1349,12 @@
       <c r="C41" s="6">
         <v>3</v>
       </c>
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1257,6 +1369,9 @@
       <c r="D42" t="s">
         <v>80</v>
       </c>
+      <c r="E42" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1271,6 +1386,9 @@
       <c r="D43" t="s">
         <v>81</v>
       </c>
+      <c r="E43" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1283,6 +1401,12 @@
         <f>0.38751610493371*0.00001</f>
         <v>3.8751610493371007E-6</v>
       </c>
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1295,6 +1419,12 @@
         <f>0.51128491182691*0.00001</f>
         <v>5.1128491182691007E-6</v>
       </c>
+      <c r="D45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1312,6 +1442,9 @@
       <c r="C47" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="D47" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1323,8 +1456,14 @@
       <c r="C48" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -1334,12 +1473,21 @@
       <c r="C49" s="7">
         <v>2320</v>
       </c>
+      <c r="D49" t="s">
+        <v>103</v>
+      </c>
+      <c r="E49" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{D4123C05-382B-4030-86ED-5C960F5B07B7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>